<commit_message>
update scripts wuth new tpm
</commit_message>
<xml_diff>
--- a/NatmiData/natmiOut_TPM/OldD0/LR-pairs_lrc2p/A2m-Lrp1.xlsx
+++ b/NatmiData/natmiOut_TPM/OldD0/LR-pairs_lrc2p/A2m-Lrp1.xlsx
@@ -552,28 +552,28 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>21.08181366666667</v>
+        <v>3.456265333333333</v>
       </c>
       <c r="N2">
-        <v>63.245441</v>
+        <v>10.368796</v>
       </c>
       <c r="O2">
-        <v>0.0571606014598545</v>
+        <v>0.009841535807677501</v>
       </c>
       <c r="P2">
-        <v>0.0571606014598545</v>
+        <v>0.0098415358076775</v>
       </c>
       <c r="Q2">
-        <v>3.778985372462222</v>
+        <v>0.6195470818844444</v>
       </c>
       <c r="R2">
-        <v>34.01086835216</v>
+        <v>5.57592373696</v>
       </c>
       <c r="S2">
-        <v>0.0571606014598545</v>
+        <v>0.009841535807677501</v>
       </c>
       <c r="T2">
-        <v>0.0571606014598545</v>
+        <v>0.0098415358076775</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -620,10 +620,10 @@
         <v>904.800446</v>
       </c>
       <c r="O3">
-        <v>0.8177496571571792</v>
+        <v>0.8587907398420774</v>
       </c>
       <c r="P3">
-        <v>0.8177496571571792</v>
+        <v>0.8587907398420773</v>
       </c>
       <c r="Q3">
         <v>54.06283198232889</v>
@@ -632,10 +632,10 @@
         <v>486.56548784096</v>
       </c>
       <c r="S3">
-        <v>0.8177496571571792</v>
+        <v>0.8587907398420774</v>
       </c>
       <c r="T3">
-        <v>0.8177496571571792</v>
+        <v>0.8587907398420773</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -682,10 +682,10 @@
         <v>138.405749</v>
       </c>
       <c r="O4">
-        <v>0.1250897413829664</v>
+        <v>0.1313677243502452</v>
       </c>
       <c r="P4">
-        <v>0.1250897413829664</v>
+        <v>0.1313677243502452</v>
       </c>
       <c r="Q4">
         <v>8.269897286915558</v>
@@ -694,10 +694,10 @@
         <v>74.42907558224</v>
       </c>
       <c r="S4">
-        <v>0.1250897413829664</v>
+        <v>0.1313677243502452</v>
       </c>
       <c r="T4">
-        <v>0.1250897413829664</v>
+        <v>0.1313677243502452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>